<commit_message>
Updating to country/region as per guidelines
</commit_message>
<xml_diff>
--- a/docs/resources/samples/table-of-contents.xlsx
+++ b/docs/resources/samples/table-of-contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26807"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\resources\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94F5F952-F706-4B4F-BF01-9FD37DFAC104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6E5E0D-3FEE-485B-AE92-22898A1335FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="75" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017 Sales" sheetId="1" r:id="rId1"/>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>Last Name</t>
-  </si>
-  <si>
-    <t>Country</t>
   </si>
   <si>
     <t>Date 1</t>
@@ -761,6 +758,9 @@
   </si>
   <si>
     <t>Smith</t>
+  </si>
+  <si>
+    <t>Country/Region</t>
   </si>
 </sst>
 </file>
@@ -43037,7 +43037,7 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{AF1391F3-A118-47AF-97FB-4DD0B18C5F3D}" name="First Name"/>
     <tableColumn id="2" xr3:uid="{2AC8F14F-3245-41B6-9D44-CECA62914261}" name="Last Name"/>
-    <tableColumn id="3" xr3:uid="{B55B595C-E751-4738-B289-4BDF4BEE3703}" name="Country"/>
+    <tableColumn id="3" xr3:uid="{B55B595C-E751-4738-B289-4BDF4BEE3703}" name="Country/Region"/>
     <tableColumn id="4" xr3:uid="{8C6B923D-09DE-4CAD-9D20-71EF32FA0C73}" name="Date 1" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{56B4A7D1-1C63-400D-B94C-B3FC6A6A024D}" name="Price"/>
     <tableColumn id="6" xr3:uid="{E360D802-7634-4C5B-AC9E-AF3DDD9F16DB}" name="Cost"/>
@@ -43056,7 +43056,7 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{AEBEC474-3394-4ECF-9DFD-CDCFD2BF7998}" name="First Name"/>
     <tableColumn id="2" xr3:uid="{E313E748-F895-497A-93ED-BA71B7C58E28}" name="Last Name"/>
-    <tableColumn id="3" xr3:uid="{5FC22027-A8E4-47A1-89CC-7E62B3EE5EAA}" name="Country"/>
+    <tableColumn id="3" xr3:uid="{5FC22027-A8E4-47A1-89CC-7E62B3EE5EAA}" name="Country/Region"/>
     <tableColumn id="4" xr3:uid="{CBF9F1B2-35F9-40B0-ABF5-75BB136D55ED}" name="Date 1" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{66AE12F6-713D-48FC-9B89-BF81A0803F70}" name="Price"/>
     <tableColumn id="6" xr3:uid="{AD2AF265-73D4-47CF-9FF6-EC0E75D64819}" name="Cost"/>
@@ -43075,7 +43075,7 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{0F9A3210-8101-48F1-8984-AEC01F8A1339}" name="First Name"/>
     <tableColumn id="2" xr3:uid="{0AE14879-9821-4F25-8E7E-AB65BCE96588}" name="Last Name"/>
-    <tableColumn id="3" xr3:uid="{F2BE05EB-BC68-4EEC-95FF-F6D490634A4B}" name="Country"/>
+    <tableColumn id="3" xr3:uid="{F2BE05EB-BC68-4EEC-95FF-F6D490634A4B}" name="Country/Region"/>
     <tableColumn id="4" xr3:uid="{12D8013A-1564-4F4A-AFF9-8EE03A62BB0A}" name="Date 1" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{6F52870C-DE0A-4A2E-BBB2-7D5D9A248713}" name="Price"/>
     <tableColumn id="6" xr3:uid="{A09F1E75-A980-47AC-BA79-1A0F6266F9EB}" name="Cost"/>
@@ -43089,9 +43089,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -43129,7 +43129,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -43235,7 +43235,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -43377,7 +43377,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -43388,22 +43388,22 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -43411,36 +43411,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2" t="e" vm="1">
         <v>#VALUE!</v>
@@ -43467,12 +43467,12 @@
         <v>33100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3" t="e" vm="2">
         <v>#VALUE!</v>
@@ -43499,12 +43499,12 @@
         <v>64848</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4" t="e" vm="3">
         <v>#VALUE!</v>
@@ -43531,12 +43531,12 @@
         <v>30940</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
       <c r="C5" t="e" vm="2">
         <v>#VALUE!</v>
@@ -43563,12 +43563,12 @@
         <v>26800</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
       </c>
       <c r="C6" t="e" vm="2">
         <v>#VALUE!</v>
@@ -43595,12 +43595,12 @@
         <v>19082</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
       </c>
       <c r="C7" t="e" vm="4">
         <v>#VALUE!</v>
@@ -43627,12 +43627,12 @@
         <v>16525</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
       </c>
       <c r="C8" t="e" vm="5">
         <v>#VALUE!</v>
@@ -43659,12 +43659,12 @@
         <v>21299</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
       </c>
       <c r="C9" t="e" vm="4">
         <v>#VALUE!</v>
@@ -43691,12 +43691,12 @@
         <v>14155</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
       </c>
       <c r="C10" t="e" vm="6">
         <v>#VALUE!</v>
@@ -43723,12 +43723,12 @@
         <v>24398</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
       </c>
       <c r="C11" t="e" vm="2">
         <v>#VALUE!</v>
@@ -43755,12 +43755,12 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
       </c>
       <c r="C12" t="e" vm="7">
         <v>#VALUE!</v>
@@ -43787,12 +43787,12 @@
         <v>57500</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
       </c>
       <c r="C13" t="e" vm="8">
         <v>#VALUE!</v>
@@ -43819,12 +43819,12 @@
         <v>11190</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
       </c>
       <c r="C14" t="e" vm="4">
         <v>#VALUE!</v>
@@ -43851,12 +43851,12 @@
         <v>33374</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
       </c>
       <c r="C15" t="e" vm="1">
         <v>#VALUE!</v>
@@ -43883,12 +43883,12 @@
         <v>56889</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
       </c>
       <c r="C16" t="e" vm="9">
         <v>#VALUE!</v>
@@ -43915,12 +43915,12 @@
         <v>33648</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
       </c>
       <c r="C17" t="e" vm="10">
         <v>#VALUE!</v>
@@ -43947,12 +43947,12 @@
         <v>7665</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
       </c>
       <c r="C18" t="e" vm="11">
         <v>#VALUE!</v>
@@ -43979,12 +43979,12 @@
         <v>34047</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
         <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
       </c>
       <c r="C19" t="e" vm="12">
         <v>#VALUE!</v>
@@ -44011,12 +44011,12 @@
         <v>18972</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
       </c>
       <c r="C20" t="e" vm="11">
         <v>#VALUE!</v>
@@ -44043,12 +44043,12 @@
         <v>12298</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
       </c>
       <c r="C21" t="e" vm="13">
         <v>#VALUE!</v>
@@ -44075,12 +44075,12 @@
         <v>26364</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
         <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
       </c>
       <c r="C22" t="e" vm="14">
         <v>#VALUE!</v>
@@ -44107,12 +44107,12 @@
         <v>18282</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
         <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>55</v>
       </c>
       <c r="C23" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44139,12 +44139,12 @@
         <v>37925</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
         <v>56</v>
-      </c>
-      <c r="B24" t="s">
-        <v>57</v>
       </c>
       <c r="C24" t="e" vm="6">
         <v>#VALUE!</v>
@@ -44171,12 +44171,12 @@
         <v>4082</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
       </c>
       <c r="C25" t="e" vm="8">
         <v>#VALUE!</v>
@@ -44203,12 +44203,12 @@
         <v>41748</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>61</v>
       </c>
       <c r="C26" t="e" vm="14">
         <v>#VALUE!</v>
@@ -44248,22 +44248,22 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -44271,36 +44271,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
       </c>
       <c r="C2" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44327,12 +44327,12 @@
         <v>11362</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
       </c>
       <c r="C3" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44359,12 +44359,12 @@
         <v>37410</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
       </c>
       <c r="C4" t="e" vm="8">
         <v>#VALUE!</v>
@@ -44391,12 +44391,12 @@
         <v>17226</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
       </c>
       <c r="C5" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44423,12 +44423,12 @@
         <v>49610</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" t="e" vm="9">
         <v>#VALUE!</v>
@@ -44455,12 +44455,12 @@
         <v>13384</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
         <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
       </c>
       <c r="C7" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44487,12 +44487,12 @@
         <v>4710</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
         <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
       </c>
       <c r="C8" t="e" vm="9">
         <v>#VALUE!</v>
@@ -44519,12 +44519,12 @@
         <v>30889</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
         <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
       </c>
       <c r="C9" t="e" vm="9">
         <v>#VALUE!</v>
@@ -44551,12 +44551,12 @@
         <v>24576</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
         <v>77</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
       </c>
       <c r="C10" t="e" vm="15">
         <v>#VALUE!</v>
@@ -44583,12 +44583,12 @@
         <v>12309</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
         <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
       </c>
       <c r="C11" t="e" vm="16">
         <v>#VALUE!</v>
@@ -44615,12 +44615,12 @@
         <v>18792</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
         <v>81</v>
-      </c>
-      <c r="B12" t="s">
-        <v>82</v>
       </c>
       <c r="C12" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44647,12 +44647,12 @@
         <v>66346</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
         <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>84</v>
       </c>
       <c r="C13" t="e" vm="17">
         <v>#VALUE!</v>
@@ -44679,12 +44679,12 @@
         <v>25740</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
         <v>85</v>
-      </c>
-      <c r="B14" t="s">
-        <v>86</v>
       </c>
       <c r="C14" t="e" vm="18">
         <v>#VALUE!</v>
@@ -44711,12 +44711,12 @@
         <v>6540</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
         <v>87</v>
-      </c>
-      <c r="B15" t="s">
-        <v>88</v>
       </c>
       <c r="C15" t="e" vm="19">
         <v>#VALUE!</v>
@@ -44743,12 +44743,12 @@
         <v>32308</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
         <v>89</v>
-      </c>
-      <c r="B16" t="s">
-        <v>90</v>
       </c>
       <c r="C16" t="e" vm="6">
         <v>#VALUE!</v>
@@ -44775,12 +44775,12 @@
         <v>16870</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
         <v>91</v>
-      </c>
-      <c r="B17" t="s">
-        <v>92</v>
       </c>
       <c r="C17" t="e" vm="9">
         <v>#VALUE!</v>
@@ -44807,12 +44807,12 @@
         <v>17423</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" t="s">
         <v>93</v>
-      </c>
-      <c r="B18" t="s">
-        <v>94</v>
       </c>
       <c r="C18" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44839,12 +44839,12 @@
         <v>14345</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
         <v>95</v>
-      </c>
-      <c r="B19" t="s">
-        <v>96</v>
       </c>
       <c r="C19" t="e" vm="12">
         <v>#VALUE!</v>
@@ -44871,12 +44871,12 @@
         <v>9732</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
         <v>97</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
       </c>
       <c r="C20" t="e" vm="20">
         <v>#VALUE!</v>
@@ -44903,12 +44903,12 @@
         <v>44560</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
         <v>99</v>
-      </c>
-      <c r="B21" t="s">
-        <v>100</v>
       </c>
       <c r="C21" t="e" vm="6">
         <v>#VALUE!</v>
@@ -44935,12 +44935,12 @@
         <v>14920</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" t="s">
         <v>101</v>
-      </c>
-      <c r="B22" t="s">
-        <v>102</v>
       </c>
       <c r="C22" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44967,12 +44967,12 @@
         <v>13794</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
         <v>103</v>
-      </c>
-      <c r="B23" t="s">
-        <v>104</v>
       </c>
       <c r="C23" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44999,12 +44999,12 @@
         <v>56964</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" t="s">
         <v>105</v>
-      </c>
-      <c r="B24" t="s">
-        <v>106</v>
       </c>
       <c r="C24" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45031,12 +45031,12 @@
         <v>18250</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
         <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
       </c>
       <c r="C25" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45063,12 +45063,12 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
         <v>109</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
       </c>
       <c r="C26" t="e" vm="9">
         <v>#VALUE!</v>
@@ -45108,22 +45108,22 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -45131,36 +45131,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
       </c>
       <c r="C2" t="e" vm="21">
         <v>#VALUE!</v>
@@ -45187,12 +45187,12 @@
         <v>64260</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>114</v>
       </c>
       <c r="C3" t="e" vm="9">
         <v>#VALUE!</v>
@@ -45219,12 +45219,12 @@
         <v>55160</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
       </c>
       <c r="C4" t="e" vm="10">
         <v>#VALUE!</v>
@@ -45251,12 +45251,12 @@
         <v>28017</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
         <v>101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
       </c>
       <c r="C5" t="e" vm="8">
         <v>#VALUE!</v>
@@ -45283,12 +45283,12 @@
         <v>21604</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
         <v>117</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
       </c>
       <c r="C6" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45315,12 +45315,12 @@
         <v>24060</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
         <v>119</v>
-      </c>
-      <c r="B7" t="s">
-        <v>120</v>
       </c>
       <c r="C7" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45347,12 +45347,12 @@
         <v>23359</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
         <v>121</v>
-      </c>
-      <c r="B8" t="s">
-        <v>122</v>
       </c>
       <c r="C8" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45379,12 +45379,12 @@
         <v>22520</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45411,12 +45411,12 @@
         <v>14248</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
         <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>125</v>
       </c>
       <c r="C10" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45443,12 +45443,12 @@
         <v>10716</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
         <v>126</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
       </c>
       <c r="C11" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45475,12 +45475,12 @@
         <v>29842</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
         <v>128</v>
-      </c>
-      <c r="B12" t="s">
-        <v>129</v>
       </c>
       <c r="C12" t="e" vm="8">
         <v>#VALUE!</v>
@@ -45507,12 +45507,12 @@
         <v>32915</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
         <v>130</v>
-      </c>
-      <c r="B13" t="s">
-        <v>131</v>
       </c>
       <c r="C13" t="e" vm="22">
         <v>#VALUE!</v>
@@ -45539,12 +45539,12 @@
         <v>9453</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
         <v>132</v>
-      </c>
-      <c r="B14" t="s">
-        <v>133</v>
       </c>
       <c r="C14" t="e" vm="23">
         <v>#VALUE!</v>
@@ -45571,12 +45571,12 @@
         <v>14416</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" t="s">
         <v>134</v>
-      </c>
-      <c r="B15" t="s">
-        <v>135</v>
       </c>
       <c r="C15" t="e" vm="24">
         <v>#VALUE!</v>
@@ -45603,12 +45603,12 @@
         <v>10660</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" t="s">
         <v>136</v>
-      </c>
-      <c r="B16" t="s">
-        <v>137</v>
       </c>
       <c r="C16" t="e" vm="9">
         <v>#VALUE!</v>
@@ -45635,12 +45635,12 @@
         <v>36416</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
         <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>74</v>
       </c>
       <c r="C17" t="e" vm="14">
         <v>#VALUE!</v>
@@ -45667,12 +45667,12 @@
         <v>55174</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
         <v>138</v>
-      </c>
-      <c r="B18" t="s">
-        <v>139</v>
       </c>
       <c r="C18" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45699,12 +45699,12 @@
         <v>33856</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" t="s">
         <v>140</v>
-      </c>
-      <c r="B19" t="s">
-        <v>141</v>
       </c>
       <c r="C19" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45731,12 +45731,12 @@
         <v>21780</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" t="s">
         <v>142</v>
-      </c>
-      <c r="B20" t="s">
-        <v>143</v>
       </c>
       <c r="C20" t="e" vm="10">
         <v>#VALUE!</v>
@@ -45763,12 +45763,12 @@
         <v>29578</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
         <v>144</v>
-      </c>
-      <c r="B21" t="s">
-        <v>145</v>
       </c>
       <c r="C21" t="e" vm="11">
         <v>#VALUE!</v>
@@ -45795,12 +45795,12 @@
         <v>24416</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C22" t="e" vm="14">
         <v>#VALUE!</v>
@@ -45827,12 +45827,12 @@
         <v>41118</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" t="s">
         <v>147</v>
-      </c>
-      <c r="B23" t="s">
-        <v>148</v>
       </c>
       <c r="C23" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45859,12 +45859,12 @@
         <v>11190</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" t="s">
         <v>149</v>
-      </c>
-      <c r="B24" t="s">
-        <v>150</v>
       </c>
       <c r="C24" t="e" vm="25">
         <v>#VALUE!</v>
@@ -45891,12 +45891,12 @@
         <v>39228</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" t="s">
         <v>151</v>
-      </c>
-      <c r="B25" t="s">
-        <v>152</v>
       </c>
       <c r="C25" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45923,12 +45923,12 @@
         <v>40710</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" t="s">
         <v>153</v>
-      </c>
-      <c r="B26" t="s">
-        <v>154</v>
       </c>
       <c r="C26" t="e" vm="24">
         <v>#VALUE!</v>

</xml_diff>

<commit_message>
Updating to country/region as per guidelines (#629)
</commit_message>
<xml_diff>
--- a/docs/resources/samples/table-of-contents.xlsx
+++ b/docs/resources/samples/table-of-contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26807"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\resources\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94F5F952-F706-4B4F-BF01-9FD37DFAC104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6E5E0D-3FEE-485B-AE92-22898A1335FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="75" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017 Sales" sheetId="1" r:id="rId1"/>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>Last Name</t>
-  </si>
-  <si>
-    <t>Country</t>
   </si>
   <si>
     <t>Date 1</t>
@@ -761,6 +758,9 @@
   </si>
   <si>
     <t>Smith</t>
+  </si>
+  <si>
+    <t>Country/Region</t>
   </si>
 </sst>
 </file>
@@ -43037,7 +43037,7 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{AF1391F3-A118-47AF-97FB-4DD0B18C5F3D}" name="First Name"/>
     <tableColumn id="2" xr3:uid="{2AC8F14F-3245-41B6-9D44-CECA62914261}" name="Last Name"/>
-    <tableColumn id="3" xr3:uid="{B55B595C-E751-4738-B289-4BDF4BEE3703}" name="Country"/>
+    <tableColumn id="3" xr3:uid="{B55B595C-E751-4738-B289-4BDF4BEE3703}" name="Country/Region"/>
     <tableColumn id="4" xr3:uid="{8C6B923D-09DE-4CAD-9D20-71EF32FA0C73}" name="Date 1" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{56B4A7D1-1C63-400D-B94C-B3FC6A6A024D}" name="Price"/>
     <tableColumn id="6" xr3:uid="{E360D802-7634-4C5B-AC9E-AF3DDD9F16DB}" name="Cost"/>
@@ -43056,7 +43056,7 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{AEBEC474-3394-4ECF-9DFD-CDCFD2BF7998}" name="First Name"/>
     <tableColumn id="2" xr3:uid="{E313E748-F895-497A-93ED-BA71B7C58E28}" name="Last Name"/>
-    <tableColumn id="3" xr3:uid="{5FC22027-A8E4-47A1-89CC-7E62B3EE5EAA}" name="Country"/>
+    <tableColumn id="3" xr3:uid="{5FC22027-A8E4-47A1-89CC-7E62B3EE5EAA}" name="Country/Region"/>
     <tableColumn id="4" xr3:uid="{CBF9F1B2-35F9-40B0-ABF5-75BB136D55ED}" name="Date 1" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{66AE12F6-713D-48FC-9B89-BF81A0803F70}" name="Price"/>
     <tableColumn id="6" xr3:uid="{AD2AF265-73D4-47CF-9FF6-EC0E75D64819}" name="Cost"/>
@@ -43075,7 +43075,7 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{0F9A3210-8101-48F1-8984-AEC01F8A1339}" name="First Name"/>
     <tableColumn id="2" xr3:uid="{0AE14879-9821-4F25-8E7E-AB65BCE96588}" name="Last Name"/>
-    <tableColumn id="3" xr3:uid="{F2BE05EB-BC68-4EEC-95FF-F6D490634A4B}" name="Country"/>
+    <tableColumn id="3" xr3:uid="{F2BE05EB-BC68-4EEC-95FF-F6D490634A4B}" name="Country/Region"/>
     <tableColumn id="4" xr3:uid="{12D8013A-1564-4F4A-AFF9-8EE03A62BB0A}" name="Date 1" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{6F52870C-DE0A-4A2E-BBB2-7D5D9A248713}" name="Price"/>
     <tableColumn id="6" xr3:uid="{A09F1E75-A980-47AC-BA79-1A0F6266F9EB}" name="Cost"/>
@@ -43089,9 +43089,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -43129,7 +43129,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -43235,7 +43235,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -43377,7 +43377,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -43388,22 +43388,22 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -43411,36 +43411,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2" t="e" vm="1">
         <v>#VALUE!</v>
@@ -43467,12 +43467,12 @@
         <v>33100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3" t="e" vm="2">
         <v>#VALUE!</v>
@@ -43499,12 +43499,12 @@
         <v>64848</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4" t="e" vm="3">
         <v>#VALUE!</v>
@@ -43531,12 +43531,12 @@
         <v>30940</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
       <c r="C5" t="e" vm="2">
         <v>#VALUE!</v>
@@ -43563,12 +43563,12 @@
         <v>26800</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
       </c>
       <c r="C6" t="e" vm="2">
         <v>#VALUE!</v>
@@ -43595,12 +43595,12 @@
         <v>19082</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
       </c>
       <c r="C7" t="e" vm="4">
         <v>#VALUE!</v>
@@ -43627,12 +43627,12 @@
         <v>16525</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
       </c>
       <c r="C8" t="e" vm="5">
         <v>#VALUE!</v>
@@ -43659,12 +43659,12 @@
         <v>21299</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
       </c>
       <c r="C9" t="e" vm="4">
         <v>#VALUE!</v>
@@ -43691,12 +43691,12 @@
         <v>14155</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
       </c>
       <c r="C10" t="e" vm="6">
         <v>#VALUE!</v>
@@ -43723,12 +43723,12 @@
         <v>24398</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
       </c>
       <c r="C11" t="e" vm="2">
         <v>#VALUE!</v>
@@ -43755,12 +43755,12 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
       </c>
       <c r="C12" t="e" vm="7">
         <v>#VALUE!</v>
@@ -43787,12 +43787,12 @@
         <v>57500</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
       </c>
       <c r="C13" t="e" vm="8">
         <v>#VALUE!</v>
@@ -43819,12 +43819,12 @@
         <v>11190</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
       </c>
       <c r="C14" t="e" vm="4">
         <v>#VALUE!</v>
@@ -43851,12 +43851,12 @@
         <v>33374</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
       </c>
       <c r="C15" t="e" vm="1">
         <v>#VALUE!</v>
@@ -43883,12 +43883,12 @@
         <v>56889</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
       </c>
       <c r="C16" t="e" vm="9">
         <v>#VALUE!</v>
@@ -43915,12 +43915,12 @@
         <v>33648</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
       </c>
       <c r="C17" t="e" vm="10">
         <v>#VALUE!</v>
@@ -43947,12 +43947,12 @@
         <v>7665</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
       </c>
       <c r="C18" t="e" vm="11">
         <v>#VALUE!</v>
@@ -43979,12 +43979,12 @@
         <v>34047</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
         <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
       </c>
       <c r="C19" t="e" vm="12">
         <v>#VALUE!</v>
@@ -44011,12 +44011,12 @@
         <v>18972</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
       </c>
       <c r="C20" t="e" vm="11">
         <v>#VALUE!</v>
@@ -44043,12 +44043,12 @@
         <v>12298</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
       </c>
       <c r="C21" t="e" vm="13">
         <v>#VALUE!</v>
@@ -44075,12 +44075,12 @@
         <v>26364</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
         <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
       </c>
       <c r="C22" t="e" vm="14">
         <v>#VALUE!</v>
@@ -44107,12 +44107,12 @@
         <v>18282</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
         <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>55</v>
       </c>
       <c r="C23" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44139,12 +44139,12 @@
         <v>37925</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
         <v>56</v>
-      </c>
-      <c r="B24" t="s">
-        <v>57</v>
       </c>
       <c r="C24" t="e" vm="6">
         <v>#VALUE!</v>
@@ -44171,12 +44171,12 @@
         <v>4082</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
       </c>
       <c r="C25" t="e" vm="8">
         <v>#VALUE!</v>
@@ -44203,12 +44203,12 @@
         <v>41748</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>61</v>
       </c>
       <c r="C26" t="e" vm="14">
         <v>#VALUE!</v>
@@ -44248,22 +44248,22 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -44271,36 +44271,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
       </c>
       <c r="C2" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44327,12 +44327,12 @@
         <v>11362</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
       </c>
       <c r="C3" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44359,12 +44359,12 @@
         <v>37410</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
       </c>
       <c r="C4" t="e" vm="8">
         <v>#VALUE!</v>
@@ -44391,12 +44391,12 @@
         <v>17226</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
       </c>
       <c r="C5" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44423,12 +44423,12 @@
         <v>49610</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" t="e" vm="9">
         <v>#VALUE!</v>
@@ -44455,12 +44455,12 @@
         <v>13384</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
         <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
       </c>
       <c r="C7" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44487,12 +44487,12 @@
         <v>4710</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
         <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
       </c>
       <c r="C8" t="e" vm="9">
         <v>#VALUE!</v>
@@ -44519,12 +44519,12 @@
         <v>30889</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
         <v>75</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
       </c>
       <c r="C9" t="e" vm="9">
         <v>#VALUE!</v>
@@ -44551,12 +44551,12 @@
         <v>24576</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
         <v>77</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
       </c>
       <c r="C10" t="e" vm="15">
         <v>#VALUE!</v>
@@ -44583,12 +44583,12 @@
         <v>12309</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
         <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
       </c>
       <c r="C11" t="e" vm="16">
         <v>#VALUE!</v>
@@ -44615,12 +44615,12 @@
         <v>18792</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
         <v>81</v>
-      </c>
-      <c r="B12" t="s">
-        <v>82</v>
       </c>
       <c r="C12" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44647,12 +44647,12 @@
         <v>66346</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
         <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>84</v>
       </c>
       <c r="C13" t="e" vm="17">
         <v>#VALUE!</v>
@@ -44679,12 +44679,12 @@
         <v>25740</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
         <v>85</v>
-      </c>
-      <c r="B14" t="s">
-        <v>86</v>
       </c>
       <c r="C14" t="e" vm="18">
         <v>#VALUE!</v>
@@ -44711,12 +44711,12 @@
         <v>6540</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
         <v>87</v>
-      </c>
-      <c r="B15" t="s">
-        <v>88</v>
       </c>
       <c r="C15" t="e" vm="19">
         <v>#VALUE!</v>
@@ -44743,12 +44743,12 @@
         <v>32308</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
         <v>89</v>
-      </c>
-      <c r="B16" t="s">
-        <v>90</v>
       </c>
       <c r="C16" t="e" vm="6">
         <v>#VALUE!</v>
@@ -44775,12 +44775,12 @@
         <v>16870</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
         <v>91</v>
-      </c>
-      <c r="B17" t="s">
-        <v>92</v>
       </c>
       <c r="C17" t="e" vm="9">
         <v>#VALUE!</v>
@@ -44807,12 +44807,12 @@
         <v>17423</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" t="s">
         <v>93</v>
-      </c>
-      <c r="B18" t="s">
-        <v>94</v>
       </c>
       <c r="C18" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44839,12 +44839,12 @@
         <v>14345</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
         <v>95</v>
-      </c>
-      <c r="B19" t="s">
-        <v>96</v>
       </c>
       <c r="C19" t="e" vm="12">
         <v>#VALUE!</v>
@@ -44871,12 +44871,12 @@
         <v>9732</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
         <v>97</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
       </c>
       <c r="C20" t="e" vm="20">
         <v>#VALUE!</v>
@@ -44903,12 +44903,12 @@
         <v>44560</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
         <v>99</v>
-      </c>
-      <c r="B21" t="s">
-        <v>100</v>
       </c>
       <c r="C21" t="e" vm="6">
         <v>#VALUE!</v>
@@ -44935,12 +44935,12 @@
         <v>14920</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" t="s">
         <v>101</v>
-      </c>
-      <c r="B22" t="s">
-        <v>102</v>
       </c>
       <c r="C22" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44967,12 +44967,12 @@
         <v>13794</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
         <v>103</v>
-      </c>
-      <c r="B23" t="s">
-        <v>104</v>
       </c>
       <c r="C23" t="e" vm="2">
         <v>#VALUE!</v>
@@ -44999,12 +44999,12 @@
         <v>56964</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" t="s">
         <v>105</v>
-      </c>
-      <c r="B24" t="s">
-        <v>106</v>
       </c>
       <c r="C24" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45031,12 +45031,12 @@
         <v>18250</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
         <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
       </c>
       <c r="C25" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45063,12 +45063,12 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
         <v>109</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
       </c>
       <c r="C26" t="e" vm="9">
         <v>#VALUE!</v>
@@ -45108,22 +45108,22 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -45131,36 +45131,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
       </c>
       <c r="C2" t="e" vm="21">
         <v>#VALUE!</v>
@@ -45187,12 +45187,12 @@
         <v>64260</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>114</v>
       </c>
       <c r="C3" t="e" vm="9">
         <v>#VALUE!</v>
@@ -45219,12 +45219,12 @@
         <v>55160</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
       </c>
       <c r="C4" t="e" vm="10">
         <v>#VALUE!</v>
@@ -45251,12 +45251,12 @@
         <v>28017</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
         <v>101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
       </c>
       <c r="C5" t="e" vm="8">
         <v>#VALUE!</v>
@@ -45283,12 +45283,12 @@
         <v>21604</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
         <v>117</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
       </c>
       <c r="C6" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45315,12 +45315,12 @@
         <v>24060</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
         <v>119</v>
-      </c>
-      <c r="B7" t="s">
-        <v>120</v>
       </c>
       <c r="C7" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45347,12 +45347,12 @@
         <v>23359</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
         <v>121</v>
-      </c>
-      <c r="B8" t="s">
-        <v>122</v>
       </c>
       <c r="C8" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45379,12 +45379,12 @@
         <v>22520</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45411,12 +45411,12 @@
         <v>14248</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
         <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>125</v>
       </c>
       <c r="C10" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45443,12 +45443,12 @@
         <v>10716</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
         <v>126</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
       </c>
       <c r="C11" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45475,12 +45475,12 @@
         <v>29842</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
         <v>128</v>
-      </c>
-      <c r="B12" t="s">
-        <v>129</v>
       </c>
       <c r="C12" t="e" vm="8">
         <v>#VALUE!</v>
@@ -45507,12 +45507,12 @@
         <v>32915</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
         <v>130</v>
-      </c>
-      <c r="B13" t="s">
-        <v>131</v>
       </c>
       <c r="C13" t="e" vm="22">
         <v>#VALUE!</v>
@@ -45539,12 +45539,12 @@
         <v>9453</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
         <v>132</v>
-      </c>
-      <c r="B14" t="s">
-        <v>133</v>
       </c>
       <c r="C14" t="e" vm="23">
         <v>#VALUE!</v>
@@ -45571,12 +45571,12 @@
         <v>14416</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" t="s">
         <v>134</v>
-      </c>
-      <c r="B15" t="s">
-        <v>135</v>
       </c>
       <c r="C15" t="e" vm="24">
         <v>#VALUE!</v>
@@ -45603,12 +45603,12 @@
         <v>10660</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" t="s">
         <v>136</v>
-      </c>
-      <c r="B16" t="s">
-        <v>137</v>
       </c>
       <c r="C16" t="e" vm="9">
         <v>#VALUE!</v>
@@ -45635,12 +45635,12 @@
         <v>36416</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
         <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>74</v>
       </c>
       <c r="C17" t="e" vm="14">
         <v>#VALUE!</v>
@@ -45667,12 +45667,12 @@
         <v>55174</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
         <v>138</v>
-      </c>
-      <c r="B18" t="s">
-        <v>139</v>
       </c>
       <c r="C18" t="e" vm="6">
         <v>#VALUE!</v>
@@ -45699,12 +45699,12 @@
         <v>33856</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" t="s">
         <v>140</v>
-      </c>
-      <c r="B19" t="s">
-        <v>141</v>
       </c>
       <c r="C19" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45731,12 +45731,12 @@
         <v>21780</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" t="s">
         <v>142</v>
-      </c>
-      <c r="B20" t="s">
-        <v>143</v>
       </c>
       <c r="C20" t="e" vm="10">
         <v>#VALUE!</v>
@@ -45763,12 +45763,12 @@
         <v>29578</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
         <v>144</v>
-      </c>
-      <c r="B21" t="s">
-        <v>145</v>
       </c>
       <c r="C21" t="e" vm="11">
         <v>#VALUE!</v>
@@ -45795,12 +45795,12 @@
         <v>24416</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C22" t="e" vm="14">
         <v>#VALUE!</v>
@@ -45827,12 +45827,12 @@
         <v>41118</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" t="s">
         <v>147</v>
-      </c>
-      <c r="B23" t="s">
-        <v>148</v>
       </c>
       <c r="C23" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45859,12 +45859,12 @@
         <v>11190</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" t="s">
         <v>149</v>
-      </c>
-      <c r="B24" t="s">
-        <v>150</v>
       </c>
       <c r="C24" t="e" vm="25">
         <v>#VALUE!</v>
@@ -45891,12 +45891,12 @@
         <v>39228</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" t="s">
         <v>151</v>
-      </c>
-      <c r="B25" t="s">
-        <v>152</v>
       </c>
       <c r="C25" t="e" vm="2">
         <v>#VALUE!</v>
@@ -45923,12 +45923,12 @@
         <v>40710</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" t="s">
         <v>153</v>
-      </c>
-      <c r="B26" t="s">
-        <v>154</v>
       </c>
       <c r="C26" t="e" vm="24">
         <v>#VALUE!</v>

</xml_diff>